<commit_message>
feat: :sparkles: Add eval data and docs
</commit_message>
<xml_diff>
--- a/8_code/ai-backend/data/test_sets/order-assistance-multiple-items-test-set.xlsx
+++ b/8_code/ai-backend/data/test_sets/order-assistance-multiple-items-test-set.xlsx
@@ -458,12 +458,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>I ordered multiple items in Order ID 2180. Can you check if each item has shipped?</t>
+          <t>I ordered a few items in Order ID 1263. Have they been shipped yet?</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'orders': [{'Product ID': 17047, 'ProductName': 'intel xeon e5 2407 processor 2.2 ghz box 10 mb smart cache', 'Category': 'CPUs', 'Category ID': 2615, 'OrderID': 2180, 'CustomerID': 335, 'OrderStatus': 'Shipped', 'ReturnEligible': False, 'ShippingDate': '2024-10-12 12:24:37.765490'}]}</t>
+          <t>{'orders': [{'Product ID': 43491, 'ProductName': 'bosch kir41af30g 122cm integrated fridge white', 'Category': 'Fridges', 'Category ID': 2623, 'OrderID': 1263, 'CustomerID': 726, 'OrderStatus': 'Shipped', 'ReturnEligible': False, 'ShippingDate': '2024-10-18 12:24:37.765490'}]}</t>
         </is>
       </c>
     </row>
@@ -475,12 +475,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>I placed an order with multiple items (Order ID 3414). Could you please tell me the shipping status of each item?</t>
+          <t>I placed Order ID 3179 a while ago. Could you please check on the shipping status of each item?</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'orders': [{'Product ID': 13551, 'ProductName': 'targus 15 15.4 inch 38.1 39.1cm rolling laptop backpack black', 'Category': 'TVs', 'Category ID': 2614, 'OrderID': 3414, 'CustomerID': 621, 'OrderStatus': 'Delivered', 'ReturnEligible': True, 'ShippingDate': '2024-10-18 12:24:37.765490'}]}</t>
+          <t>{'orders': [{'Product ID': 46508, 'ProductName': 'liebherr k hlschrankl premium mit biofresh kbpes 4354', 'Category': 'Fridges', 'Category ID': 2623, 'OrderID': 3179, 'CustomerID': 2161, 'OrderStatus': 'Cancelled', 'ReturnEligible': False, 'ShippingDate': '2024-09-29 12:24:37.765490'}]}</t>
         </is>
       </c>
     </row>
@@ -492,12 +492,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Order 2445 has several items. Have they all shipped yet?</t>
+          <t>Order ID 2193 contains several items. Can you tell me if each one has shipped?</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'orders': [{'Product ID': 12351, 'ProductName': 'panasonic tx 77ez1002b 77 smart 4k ultra hdr oled tv', 'Category': 'TVs', 'Category ID': 2614, 'OrderID': 2445, 'CustomerID': 1217, 'OrderStatus': 'Delivered', 'ReturnEligible': True, 'ShippingDate': '2024-10-01 12:24:37.765490'}]}</t>
+          <t>{'orders': [{'Product ID': 16185, 'ProductName': 'hp intel xeon e7530 1.866ghz 12mb l3 processor', 'Category': 'CPUs', 'Category ID': 2615, 'OrderID': 2193, 'CustomerID': 2408, 'OrderStatus': 'Pending', 'ReturnEligible': False, 'ShippingDate': '2024-10-26 12:24:37.765490'}]}</t>
         </is>
       </c>
     </row>
@@ -509,12 +509,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>I'd like to know the shipping status for each item in Order ID 1933, as it contains multiple items.</t>
+          <t>In Order ID 1182, I purchased multiple items. I'd like to know the shipping status for each of them.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'orders': [{'Product ID': 10397, 'ProductName': 'sony kd43xf8505bu 43 4k hdr smart led tv', 'Category': 'TVs', 'Category ID': 2614, 'OrderID': 1933, 'CustomerID': 361, 'OrderStatus': 'Pending', 'ReturnEligible': False, 'ShippingDate': '2024-10-11 12:24:37.765490'}]}</t>
+          <t>{'orders': [{'Product ID': 44483, 'ProductName': 'zanussi zba15021sv integrated fridge', 'Category': 'Fridges', 'Category ID': 2623, 'OrderID': 1182, 'CustomerID': 193, 'OrderStatus': 'Pending', 'ReturnEligible': False, 'ShippingDate': '2024-10-05 12:24:37.765490'}]}</t>
         </is>
       </c>
     </row>
@@ -526,12 +526,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Regarding Order 1699, which includes multiple items, could you provide an update on the shipping status of each one?</t>
+          <t>I have multiple items under Order ID 1384. Can you check the shipping status for each item, please?</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'orders': [{'Product ID': 14761, 'ProductName': 'intel core i5 3210m processor 3m cache up to 3.10 ghz', 'Category': 'CPUs', 'Category ID': 2615, 'OrderID': 1699, 'CustomerID': 630, 'OrderStatus': 'Pending', 'ReturnEligible': False, 'ShippingDate': '2024-10-20 12:24:37.765490'}]}</t>
+          <t>{'orders': [{'Product ID': 42483, 'ProductName': 'siemens k hl gefrier k hl kombination wei kg39vvw31 eek a', 'Category': 'Fridge Freezers', 'Category ID': 2622, 'OrderID': 1384, 'CustomerID': 2059, 'OrderStatus': 'Pending', 'ReturnEligible': False, 'ShippingDate': '2024-10-08 12:24:37.765490'}]}</t>
         </is>
       </c>
     </row>
@@ -543,12 +543,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Can you tell me if all the items in Order ID 2430 have been shipped? It was a multi-item order.</t>
+          <t>I ordered multiple items in Order ID 1530. Can you check if each item has shipped?</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'orders': [{'Product ID': 14586, 'ProductName': 'intel xeon 1660v43 20ghz lga2011320mb cache', 'Category': 'CPUs', 'Category ID': 2615, 'OrderID': 2430, 'CustomerID': 1698, 'OrderStatus': 'Shipped', 'ReturnEligible': False, 'ShippingDate': '2024-10-19 12:24:37.765490'}]}</t>
+          <t>{'orders': [{'Product ID': 46062, 'ProductName': 'bosch k hlger t kil82ad40', 'Category': 'Fridges', 'Category ID': 2623, 'OrderID': 2830, 'CustomerID': 1349, 'OrderStatus': 'Shipped', 'ReturnEligible': False, 'ShippingDate': '2024-10-09 12:24:37.765490'}]}</t>
         </is>
       </c>
     </row>
@@ -560,12 +560,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>I have a multi-item order, Order ID 1243.  I'd like to check the shipping status for each item individually.</t>
+          <t>I placed an order with multiple items (Order ID 3183). Could you please tell me the shipping status of each item?</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'orders': [{'Product ID': 12531, 'ProductName': 'toshiba 43u6863db led hdr 4k ultra hd smart tv 43 with freeview hd freeview play black', 'Category': 'TVs', 'Category ID': 2614, 'OrderID': 1243, 'CustomerID': 1706, 'OrderStatus': 'Delivered', 'ReturnEligible': False, 'ShippingDate': '2024-10-15 12:24:37.765490'}]}</t>
+          <t>{'orders': [{'Product ID': 16829, 'ProductName': 'intel xeon e7340 processor 2.4 ghz box 8 mb l2', 'Category': 'CPUs', 'Category ID': 2615, 'OrderID': 2946, 'CustomerID': 119, 'OrderStatus': 'Shipped', 'ReturnEligible': False, 'ShippingDate': '2024-10-13 12:24:37.765490'}]}</t>
         </is>
       </c>
     </row>
@@ -577,12 +577,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>For Order ID 1282, I ordered several items. Could you please check if they have all shipped?</t>
+          <t>Order 1113 has several items. Have they all shipped yet?</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'orders': [{'Product ID': 17055, 'ProductName': 'hewlett packard enterprise dl360p gen8 intel xeon e5 2670 fio kit 2.6ghz 20mb l3 processor', 'Category': 'CPUs', 'Category ID': 2615, 'OrderID': 1282, 'CustomerID': 462, 'OrderStatus': 'Shipped', 'ReturnEligible': False, 'ShippingDate': '2024-10-01 12:24:37.765490'}]}</t>
+          <t>{'orders': [{'Product ID': 34428, 'ProductName': 'bosch waw32540', 'Category': 'Washing Machines', 'Category ID': 2620, 'OrderID': 2728, 'CustomerID': 294, 'OrderStatus': 'Cancelled', 'ReturnEligible': False, 'ShippingDate': '2024-10-13 12:24:37.765490'}]}</t>
         </is>
       </c>
     </row>
@@ -594,12 +594,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>In Order ID 2365, I purchased multiple items. Could you tell me if each item has been shipped yet?</t>
+          <t>I'd like to know the shipping status for each item in Order ID 1842. It contains multiple items.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'orders': [{'Product ID': 45932, 'ProductName': 'bosch kil52ad40 k hlger t integrierbar', 'Category': 'Fridges', 'Category ID': 2623, 'OrderID': 2365, 'CustomerID': 1020, 'OrderStatus': 'Cancelled', 'ReturnEligible': False, 'ShippingDate': '2024-10-25 12:24:37.765490'}]}</t>
+          <t>{'orders': [{'Product ID': 16843, 'ProductName': 'hewlett packard enterprise amd opteron 2352 2.1ghz 2mb l3 processor', 'Category': 'CPUs', 'Category ID': 2615, 'OrderID': 1753, 'CustomerID': 1584, 'OrderStatus': 'Shipped', 'ReturnEligible': False, 'ShippingDate': '2024-10-25 12:24:37.765490'}]}</t>
         </is>
       </c>
     </row>
@@ -611,12 +611,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>I'm checking on the shipping status of each item in Order 1959. It was a multiple item order.</t>
+          <t>Can you tell me if everything in Order 1948 has shipped? There are multiple items on this order.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'orders': [{'Product ID': 12893, 'ProductName': '43 thomson 43uc6306', 'Category': 'TVs', 'Category ID': 2614, 'OrderID': 1959, 'CustomerID': 1882, 'OrderStatus': 'Shipped', 'ReturnEligible': False, 'ShippingDate': '2024-10-23 12:24:37.765490'}]}</t>
+          <t>{'orders': [{'Product ID': 43969, 'ProductName': 'bosch kil22vs30g serie 4 built in single door fridges 88cm height with ice box white', 'Category': 'Fridges', 'Category ID': 2623, 'OrderID': 1087, 'CustomerID': 1040, 'OrderStatus': 'Cancelled', 'ReturnEligible': False, 'ShippingDate': '2024-10-25 12:24:37.765490'}]}</t>
         </is>
       </c>
     </row>

</xml_diff>